<commit_message>
updated documentation with videos
</commit_message>
<xml_diff>
--- a/doc/OPC_Jobs_Proto.xlsx
+++ b/doc/OPC_Jobs_Proto.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roa2\Höhere Fachschule für Technik Mittelland\Makroprojekt - General\F6_MPS\GIT\rcll-mps-stations\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\rcll-mps-stations\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="46" documentId="B4EC4288D6C48A2ACD671C606D6C965D4641ADC3" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{17E2AA6B-668A-467E-8DAB-F6BE2ACC7587}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{942381F7-BD85-4FFC-8D95-5BA42030AFC0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30000" windowHeight="15650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30000" windowHeight="15645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OPCJobs" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="62">
   <si>
     <t>Reset</t>
   </si>
@@ -172,30 +172,6 @@
   </si>
   <si>
     <t>SSTask</t>
-  </si>
-  <si>
-    <t>Sobald das Busy-Signal von der MPS wieder auf den Outputregistern(MPS) zurückkommt</t>
-  </si>
-  <si>
-    <t>muss es zurückgesetzt werden damit ich auch eine identische neue Action erkennen könnte.</t>
-  </si>
-  <si>
-    <t>Dann ist das Ready Signal (war zwar schon vorgesehen) nun definiert.</t>
-  </si>
-  <si>
-    <t>Dies wird MPS seitig gesetzt, bei Band-Operationen, sofern das Produkt fertig abholbereit in der</t>
-  </si>
-  <si>
-    <t>Output-Lichtschranke steht. (ready). Der Job/Action ist erst beendet, sobald dies abgeholt wurde</t>
-  </si>
-  <si>
-    <t>(Lichtschranke frei), und erst jetzt wird Busy zurückgesetzt. Selbstredend kann auch nur eine Aktion</t>
-  </si>
-  <si>
-    <t>gleichzeitig verarbeitet werden (ist ja dasselbe Band).</t>
-  </si>
-  <si>
-    <t>Ein Queuing müsste falls gewünscht auf dem Edison passieren.</t>
   </si>
   <si>
     <t>not implemented</t>
@@ -230,6 +206,12 @@
   </si>
   <si>
     <t>Enable Bit for starting a job</t>
+  </si>
+  <si>
+    <t>Busy Status while working</t>
+  </si>
+  <si>
+    <t>Basic Registers for general Jobs (MachineType, Lights)</t>
   </si>
 </sst>
 </file>
@@ -427,47 +409,47 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -786,34 +768,34 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S41"/>
+  <dimension ref="A1:S40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24:E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
-    <col min="2" max="2" width="13.81640625" customWidth="1"/>
-    <col min="3" max="3" width="7.54296875" customWidth="1"/>
-    <col min="4" max="4" width="15.81640625" customWidth="1"/>
-    <col min="5" max="5" width="9.1796875" customWidth="1"/>
-    <col min="6" max="6" width="10.54296875" customWidth="1"/>
-    <col min="7" max="7" width="11.1796875" customWidth="1"/>
-    <col min="8" max="15" width="2.1796875" style="9" customWidth="1"/>
-    <col min="16" max="16" width="9.1796875" customWidth="1"/>
-    <col min="17" max="17" width="17.81640625" customWidth="1"/>
-    <col min="18" max="19" width="8.1796875" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" customWidth="1"/>
+    <col min="8" max="15" width="2.140625" style="9" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" customWidth="1"/>
+    <col min="17" max="17" width="17.85546875" customWidth="1"/>
+    <col min="18" max="19" width="8.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" ht="3.65" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:19" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="3.6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:19" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -823,47 +805,47 @@
       <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="D3" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="35" t="s">
-        <v>65</v>
-      </c>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="36"/>
-      <c r="L3" s="36"/>
-      <c r="M3" s="36"/>
-      <c r="N3" s="36"/>
-      <c r="O3" s="37"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="32"/>
+      <c r="O3" s="33"/>
       <c r="P3" s="4" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="Q3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="R3" s="33" t="s">
-        <v>60</v>
-      </c>
-      <c r="S3" s="34"/>
-    </row>
-    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="R3" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="S3" s="26"/>
+    </row>
+    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="35" t="s">
+      <c r="D4" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="37"/>
-      <c r="F4" s="35" t="s">
+      <c r="E4" s="33"/>
+      <c r="F4" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="37"/>
+      <c r="G4" s="33"/>
       <c r="H4" s="24">
         <v>7</v>
       </c>
@@ -891,26 +873,26 @@
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
       <c r="R4" s="4" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="S4" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" s="1" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" s="1" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="37"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="33"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="10"/>
       <c r="K5" s="10"/>
       <c r="L5" s="10" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="M5" s="10" t="s">
         <v>12</v>
@@ -924,13 +906,13 @@
       <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
       <c r="R5" s="4" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="S5" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>15</v>
       </c>
@@ -940,10 +922,10 @@
       <c r="C6" s="7">
         <v>0</v>
       </c>
-      <c r="D6" s="25"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="26"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="28"/>
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
@@ -956,7 +938,7 @@
       <c r="Q6" s="4"/>
       <c r="S6" s="17"/>
     </row>
-    <row r="7" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>15</v>
       </c>
@@ -966,10 +948,10 @@
       <c r="C7" s="7">
         <v>10</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="26"/>
+      <c r="E7" s="28"/>
       <c r="F7" s="22"/>
       <c r="G7" s="23"/>
       <c r="H7" s="11"/>
@@ -984,7 +966,7 @@
       <c r="Q7" s="4"/>
       <c r="S7" s="17"/>
     </row>
-    <row r="8" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>19</v>
       </c>
@@ -994,10 +976,10 @@
       <c r="C8" s="16">
         <v>20</v>
       </c>
-      <c r="D8" s="25"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="26"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="28"/>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
@@ -1010,7 +992,7 @@
       <c r="Q8" s="4"/>
       <c r="S8" s="17"/>
     </row>
-    <row r="9" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="6" t="s">
         <v>21</v>
@@ -1018,14 +1000,14 @@
       <c r="C9" s="21">
         <v>21</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="26"/>
-      <c r="F9" s="25" t="s">
+      <c r="E9" s="28"/>
+      <c r="F9" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="26"/>
+      <c r="G9" s="28"/>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
@@ -1040,7 +1022,7 @@
       </c>
       <c r="S9" s="17"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="6" t="s">
         <v>25</v>
@@ -1048,14 +1030,14 @@
       <c r="C10" s="16">
         <v>22</v>
       </c>
-      <c r="D10" s="25" t="s">
+      <c r="D10" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="26"/>
-      <c r="F10" s="25" t="s">
+      <c r="E10" s="28"/>
+      <c r="F10" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="G10" s="26"/>
+      <c r="G10" s="28"/>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
@@ -1070,7 +1052,7 @@
       </c>
       <c r="S10" s="17"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="6" t="s">
         <v>26</v>
@@ -1078,14 +1060,14 @@
       <c r="C11" s="16">
         <v>23</v>
       </c>
-      <c r="D11" s="25" t="s">
+      <c r="D11" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="26"/>
-      <c r="F11" s="25" t="s">
+      <c r="E11" s="28"/>
+      <c r="F11" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="26"/>
+      <c r="G11" s="28"/>
       <c r="H11" s="8"/>
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
@@ -1100,7 +1082,7 @@
       </c>
       <c r="S11" s="18"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>1</v>
       </c>
@@ -1110,10 +1092,10 @@
       <c r="C12" s="7">
         <v>100</v>
       </c>
-      <c r="D12" s="25"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="26"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="28"/>
       <c r="H12" s="11"/>
       <c r="I12" s="11"/>
       <c r="J12" s="11"/>
@@ -1126,7 +1108,7 @@
       <c r="Q12" s="4"/>
       <c r="S12" s="17"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="6" t="s">
         <v>27</v>
@@ -1134,12 +1116,12 @@
       <c r="C13" s="7">
         <v>101</v>
       </c>
-      <c r="D13" s="25" t="s">
+      <c r="D13" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="26"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="26"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="28"/>
       <c r="H13" s="11"/>
       <c r="I13" s="11"/>
       <c r="J13" s="11"/>
@@ -1154,7 +1136,7 @@
       </c>
       <c r="S13" s="18"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="B14" s="15" t="s">
         <v>30</v>
@@ -1162,14 +1144,14 @@
       <c r="C14" s="16">
         <v>102</v>
       </c>
-      <c r="D14" s="31" t="s">
+      <c r="D14" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="E14" s="32"/>
-      <c r="F14" s="29" t="s">
+      <c r="E14" s="30"/>
+      <c r="F14" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="G14" s="30"/>
+      <c r="G14" s="36"/>
       <c r="H14" s="14"/>
       <c r="I14" s="14"/>
       <c r="J14" s="14"/>
@@ -1184,7 +1166,7 @@
       </c>
       <c r="S14" s="17"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>34</v>
       </c>
@@ -1194,10 +1176,10 @@
       <c r="C15" s="7">
         <v>200</v>
       </c>
-      <c r="D15" s="25"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="26"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="28"/>
       <c r="H15" s="11"/>
       <c r="I15" s="11"/>
       <c r="J15" s="11"/>
@@ -1210,7 +1192,7 @@
       <c r="Q15" s="4"/>
       <c r="S15" s="17"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="6" t="s">
         <v>35</v>
@@ -1218,12 +1200,12 @@
       <c r="C16" s="7">
         <v>201</v>
       </c>
-      <c r="D16" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="E16" s="26"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="26"/>
+      <c r="D16" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" s="28"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="28"/>
       <c r="H16" s="11"/>
       <c r="I16" s="11"/>
       <c r="J16" s="11"/>
@@ -1236,7 +1218,7 @@
       <c r="Q16" s="4"/>
       <c r="S16" s="18"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="6" t="s">
         <v>30</v>
@@ -1244,14 +1226,14 @@
       <c r="C17" s="7">
         <v>202</v>
       </c>
-      <c r="D17" s="31" t="s">
+      <c r="D17" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="E17" s="32"/>
-      <c r="F17" s="29" t="s">
+      <c r="E17" s="30"/>
+      <c r="F17" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="G17" s="30"/>
+      <c r="G17" s="36"/>
       <c r="H17" s="11"/>
       <c r="I17" s="11"/>
       <c r="J17" s="11"/>
@@ -1266,7 +1248,7 @@
       </c>
       <c r="S17" s="17"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="6" t="s">
         <v>38</v>
@@ -1274,12 +1256,12 @@
       <c r="C18" s="7">
         <v>203</v>
       </c>
-      <c r="D18" s="25" t="s">
+      <c r="D18" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="E18" s="26"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="26"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="28"/>
       <c r="H18" s="11"/>
       <c r="I18" s="11"/>
       <c r="J18" s="11"/>
@@ -1294,7 +1276,7 @@
       </c>
       <c r="S18" s="17"/>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>2</v>
       </c>
@@ -1304,10 +1286,10 @@
       <c r="C19" s="7">
         <v>300</v>
       </c>
-      <c r="D19" s="25"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="26"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="28"/>
       <c r="H19" s="11"/>
       <c r="I19" s="11"/>
       <c r="J19" s="11"/>
@@ -1320,7 +1302,7 @@
       <c r="Q19" s="4"/>
       <c r="S19" s="17"/>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="6" t="s">
         <v>30</v>
@@ -1328,14 +1310,14 @@
       <c r="C20" s="7">
         <v>302</v>
       </c>
-      <c r="D20" s="31" t="s">
+      <c r="D20" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="32"/>
-      <c r="F20" s="29" t="s">
+      <c r="E20" s="30"/>
+      <c r="F20" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="G20" s="30"/>
+      <c r="G20" s="36"/>
       <c r="H20" s="11"/>
       <c r="I20" s="11"/>
       <c r="J20" s="11"/>
@@ -1350,7 +1332,7 @@
       </c>
       <c r="S20" s="17"/>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="6" t="s">
         <v>40</v>
@@ -1358,12 +1340,12 @@
       <c r="C21" s="16">
         <v>301</v>
       </c>
-      <c r="D21" s="31" t="s">
+      <c r="D21" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="E21" s="32"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="26"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="28"/>
       <c r="H21" s="11"/>
       <c r="I21" s="11"/>
       <c r="J21" s="11"/>
@@ -1378,14 +1360,14 @@
       </c>
       <c r="S21" s="17"/>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="6"/>
       <c r="C22" s="7"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="26"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="28"/>
       <c r="H22" s="11"/>
       <c r="I22" s="11"/>
       <c r="J22" s="11"/>
@@ -1398,7 +1380,7 @@
       <c r="Q22" s="4"/>
       <c r="S22" s="17"/>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>3</v>
       </c>
@@ -1408,10 +1390,10 @@
       <c r="C23" s="7">
         <v>400</v>
       </c>
-      <c r="D23" s="25"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="26"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="28"/>
       <c r="H23" s="11"/>
       <c r="I23" s="11"/>
       <c r="J23" s="11"/>
@@ -1424,7 +1406,7 @@
       <c r="Q23" s="4"/>
       <c r="S23" s="17"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="6" t="s">
         <v>43</v>
@@ -1432,12 +1414,12 @@
       <c r="C24" s="7">
         <v>401</v>
       </c>
-      <c r="D24" s="25" t="s">
+      <c r="D24" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="E24" s="26"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="28"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="38"/>
       <c r="H24" s="11"/>
       <c r="I24" s="11"/>
       <c r="J24" s="11"/>
@@ -1452,7 +1434,7 @@
       </c>
       <c r="S24" s="17"/>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>45</v>
       </c>
@@ -1462,10 +1444,10 @@
       <c r="C25" s="7">
         <v>500</v>
       </c>
-      <c r="D25" s="25"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="25"/>
-      <c r="G25" s="26"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="28"/>
       <c r="H25" s="11"/>
       <c r="I25" s="11"/>
       <c r="J25" s="11"/>
@@ -1478,7 +1460,7 @@
       <c r="Q25" s="4"/>
       <c r="S25" s="17"/>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="6" t="s">
         <v>46</v>
@@ -1486,12 +1468,12 @@
       <c r="C26" s="7">
         <v>501</v>
       </c>
-      <c r="D26" s="25" t="s">
+      <c r="D26" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="E26" s="26"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="26"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="28"/>
       <c r="H26" s="11"/>
       <c r="I26" s="11"/>
       <c r="J26" s="11"/>
@@ -1506,14 +1488,14 @@
       </c>
       <c r="S26" s="17"/>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="7"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="26"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="28"/>
       <c r="H27" s="8"/>
       <c r="I27" s="8"/>
       <c r="J27" s="8"/>
@@ -1526,14 +1508,14 @@
       <c r="Q27" s="4"/>
       <c r="S27" s="17"/>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="6"/>
       <c r="C28" s="7"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="26"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="28"/>
       <c r="H28" s="8"/>
       <c r="I28" s="8"/>
       <c r="J28" s="8"/>
@@ -1546,91 +1528,67 @@
       <c r="Q28" s="4"/>
       <c r="S28" s="17"/>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D29" s="2"/>
       <c r="S29" s="19"/>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="20"/>
       <c r="S30" s="19"/>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A31" s="20"/>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A31" s="20" t="s">
+        <v>59</v>
+      </c>
       <c r="S31" s="19"/>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="S32" s="19"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A33" s="20" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="20"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="20" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="20"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A36" s="20" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A37" s="20" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A38" s="20" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A39" s="20" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A40" s="20" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A41" s="20" t="s">
-        <v>56</v>
-      </c>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="20"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="20"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="20"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="20"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="H3:O3"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
     <mergeCell ref="F15:G15"/>
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="F21:G21"/>
@@ -1647,20 +1605,28 @@
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="H3:O3"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F14:G14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="75" orientation="landscape" r:id="rId1"/>
@@ -1668,15 +1634,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100CA7F42331C2C26418517DD699E6CB751" ma:contentTypeVersion="8" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="2144a4f294ff69055376aff841bdaa8a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8e441a56-0832-4542-9714-47bfe0559f5f" xmlns:ns3="c1bd8b98-cc9e-46a6-b71b-104d794fef93" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4106c1069881d73dc50bd56f9b52ae75" ns2:_="" ns3:_="">
     <xsd:import namespace="8e441a56-0832-4542-9714-47bfe0559f5f"/>
@@ -1867,6 +1824,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1874,14 +1840,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48FFC07A-B65A-427B-963B-1F060EF78D23}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F77780E-A18D-4A5C-A363-627F96E03E5F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1896,6 +1854,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48FFC07A-B65A-427B-963B-1F060EF78D23}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
adaption to the very new PLC from Festo with Firmware Version 1.1.18
</commit_message>
<xml_diff>
--- a/doc/OPC_Jobs_Proto.xlsx
+++ b/doc/OPC_Jobs_Proto.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\rcll-mps-stations\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{942381F7-BD85-4FFC-8D95-5BA42030AFC0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F159CF2-5124-46C8-B4A9-0CD619629161}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30000" windowHeight="15645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12744" yWindow="5916" windowWidth="23040" windowHeight="13884" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OPCJobs" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="63">
   <si>
     <t>Reset</t>
   </si>
@@ -212,6 +212,9 @@
   </si>
   <si>
     <t>Basic Registers for general Jobs (MachineType, Lights)</t>
+  </si>
+  <si>
+    <t>Action Registers for machine specific Jobs (Band, Cylinders)</t>
   </si>
 </sst>
 </file>
@@ -357,7 +360,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -391,9 +394,8 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -409,23 +411,35 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -438,18 +452,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -770,32 +772,32 @@
   </sheetPr>
   <dimension ref="A1:S40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24:E24"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" customWidth="1"/>
-    <col min="3" max="3" width="7.5703125" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" customWidth="1"/>
-    <col min="8" max="15" width="2.140625" style="9" customWidth="1"/>
-    <col min="16" max="16" width="9.140625" customWidth="1"/>
-    <col min="17" max="17" width="17.85546875" customWidth="1"/>
-    <col min="18" max="19" width="8.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" customWidth="1"/>
+    <col min="3" max="3" width="7.5546875" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" customWidth="1"/>
+    <col min="6" max="6" width="10.5546875" customWidth="1"/>
+    <col min="7" max="7" width="11.109375" customWidth="1"/>
+    <col min="8" max="15" width="2.109375" style="9" customWidth="1"/>
+    <col min="16" max="16" width="9.109375" customWidth="1"/>
+    <col min="17" max="17" width="17.88671875" customWidth="1"/>
+    <col min="18" max="19" width="8.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="3.6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:19" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="3.6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:19" ht="29.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -805,69 +807,69 @@
       <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="34" t="s">
+      <c r="D3" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="31" t="s">
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="32"/>
-      <c r="M3" s="32"/>
-      <c r="N3" s="32"/>
-      <c r="O3" s="33"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="35"/>
+      <c r="O3" s="36"/>
       <c r="P3" s="4" t="s">
         <v>58</v>
       </c>
       <c r="Q3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="R3" s="25" t="s">
+      <c r="R3" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="S3" s="26"/>
-    </row>
-    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S3" s="33"/>
+    </row>
+    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="33"/>
-      <c r="F4" s="31" t="s">
+      <c r="E4" s="36"/>
+      <c r="F4" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="33"/>
-      <c r="H4" s="24">
+      <c r="G4" s="36"/>
+      <c r="H4" s="23">
         <v>7</v>
       </c>
-      <c r="I4" s="24">
+      <c r="I4" s="23">
         <v>6</v>
       </c>
-      <c r="J4" s="24">
+      <c r="J4" s="23">
         <v>5</v>
       </c>
-      <c r="K4" s="24">
+      <c r="K4" s="23">
         <v>4</v>
       </c>
-      <c r="L4" s="24">
+      <c r="L4" s="23">
         <v>3</v>
       </c>
-      <c r="M4" s="24">
+      <c r="M4" s="23">
         <v>2</v>
       </c>
-      <c r="N4" s="24">
+      <c r="N4" s="23">
         <v>1</v>
       </c>
-      <c r="O4" s="24">
+      <c r="O4" s="23">
         <v>0</v>
       </c>
       <c r="P4" s="4"/>
@@ -879,14 +881,14 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:19" s="1" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" s="1" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="33"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="36"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="10"/>
@@ -912,7 +914,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>15</v>
       </c>
@@ -922,10 +924,10 @@
       <c r="C6" s="7">
         <v>0</v>
       </c>
-      <c r="D6" s="27"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="28"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="25"/>
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
@@ -938,7 +940,7 @@
       <c r="Q6" s="4"/>
       <c r="S6" s="17"/>
     </row>
-    <row r="7" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>15</v>
       </c>
@@ -948,12 +950,12 @@
       <c r="C7" s="7">
         <v>10</v>
       </c>
-      <c r="D7" s="27" t="s">
+      <c r="D7" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="28"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="23"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="22"/>
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
       <c r="J7" s="11"/>
@@ -966,7 +968,7 @@
       <c r="Q7" s="4"/>
       <c r="S7" s="17"/>
     </row>
-    <row r="8" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>19</v>
       </c>
@@ -976,10 +978,10 @@
       <c r="C8" s="16">
         <v>20</v>
       </c>
-      <c r="D8" s="27"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="28"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="25"/>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
@@ -992,22 +994,22 @@
       <c r="Q8" s="4"/>
       <c r="S8" s="17"/>
     </row>
-    <row r="9" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="21">
+      <c r="C9" s="20">
         <v>21</v>
       </c>
-      <c r="D9" s="27" t="s">
+      <c r="D9" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="28"/>
-      <c r="F9" s="27" t="s">
+      <c r="E9" s="25"/>
+      <c r="F9" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="28"/>
+      <c r="G9" s="25"/>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
@@ -1022,7 +1024,7 @@
       </c>
       <c r="S9" s="17"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="6" t="s">
         <v>25</v>
@@ -1030,14 +1032,14 @@
       <c r="C10" s="16">
         <v>22</v>
       </c>
-      <c r="D10" s="27" t="s">
+      <c r="D10" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="28"/>
-      <c r="F10" s="27" t="s">
+      <c r="E10" s="25"/>
+      <c r="F10" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="G10" s="28"/>
+      <c r="G10" s="25"/>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
@@ -1052,7 +1054,7 @@
       </c>
       <c r="S10" s="17"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="6" t="s">
         <v>26</v>
@@ -1060,14 +1062,14 @@
       <c r="C11" s="16">
         <v>23</v>
       </c>
-      <c r="D11" s="27" t="s">
+      <c r="D11" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="28"/>
-      <c r="F11" s="27" t="s">
+      <c r="E11" s="25"/>
+      <c r="F11" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="28"/>
+      <c r="G11" s="25"/>
       <c r="H11" s="8"/>
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
@@ -1082,7 +1084,7 @@
       </c>
       <c r="S11" s="18"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>1</v>
       </c>
@@ -1092,10 +1094,10 @@
       <c r="C12" s="7">
         <v>100</v>
       </c>
-      <c r="D12" s="27"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="28"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="25"/>
       <c r="H12" s="11"/>
       <c r="I12" s="11"/>
       <c r="J12" s="11"/>
@@ -1108,7 +1110,7 @@
       <c r="Q12" s="4"/>
       <c r="S12" s="17"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="6" t="s">
         <v>27</v>
@@ -1116,12 +1118,12 @@
       <c r="C13" s="7">
         <v>101</v>
       </c>
-      <c r="D13" s="27" t="s">
+      <c r="D13" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="28"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="28"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="25"/>
       <c r="H13" s="11"/>
       <c r="I13" s="11"/>
       <c r="J13" s="11"/>
@@ -1136,7 +1138,7 @@
       </c>
       <c r="S13" s="18"/>
     </row>
-    <row r="14" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="12"/>
       <c r="B14" s="15" t="s">
         <v>30</v>
@@ -1144,14 +1146,14 @@
       <c r="C14" s="16">
         <v>102</v>
       </c>
-      <c r="D14" s="29" t="s">
+      <c r="D14" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="E14" s="30"/>
-      <c r="F14" s="35" t="s">
+      <c r="E14" s="31"/>
+      <c r="F14" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G14" s="36"/>
+      <c r="G14" s="29"/>
       <c r="H14" s="14"/>
       <c r="I14" s="14"/>
       <c r="J14" s="14"/>
@@ -1166,7 +1168,7 @@
       </c>
       <c r="S14" s="17"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>34</v>
       </c>
@@ -1176,10 +1178,10 @@
       <c r="C15" s="7">
         <v>200</v>
       </c>
-      <c r="D15" s="27"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="28"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="25"/>
       <c r="H15" s="11"/>
       <c r="I15" s="11"/>
       <c r="J15" s="11"/>
@@ -1192,7 +1194,7 @@
       <c r="Q15" s="4"/>
       <c r="S15" s="17"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="6" t="s">
         <v>35</v>
@@ -1200,12 +1202,12 @@
       <c r="C16" s="7">
         <v>201</v>
       </c>
-      <c r="D16" s="27" t="s">
+      <c r="D16" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="E16" s="28"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="28"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="25"/>
       <c r="H16" s="11"/>
       <c r="I16" s="11"/>
       <c r="J16" s="11"/>
@@ -1218,7 +1220,7 @@
       <c r="Q16" s="4"/>
       <c r="S16" s="18"/>
     </row>
-    <row r="17" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
       <c r="B17" s="6" t="s">
         <v>30</v>
@@ -1226,14 +1228,14 @@
       <c r="C17" s="7">
         <v>202</v>
       </c>
-      <c r="D17" s="29" t="s">
+      <c r="D17" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="E17" s="30"/>
-      <c r="F17" s="35" t="s">
+      <c r="E17" s="31"/>
+      <c r="F17" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G17" s="36"/>
+      <c r="G17" s="29"/>
       <c r="H17" s="11"/>
       <c r="I17" s="11"/>
       <c r="J17" s="11"/>
@@ -1248,7 +1250,7 @@
       </c>
       <c r="S17" s="17"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="6" t="s">
         <v>38</v>
@@ -1256,12 +1258,12 @@
       <c r="C18" s="7">
         <v>203</v>
       </c>
-      <c r="D18" s="27" t="s">
+      <c r="D18" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="E18" s="28"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="28"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="25"/>
       <c r="H18" s="11"/>
       <c r="I18" s="11"/>
       <c r="J18" s="11"/>
@@ -1276,7 +1278,7 @@
       </c>
       <c r="S18" s="17"/>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>2</v>
       </c>
@@ -1286,10 +1288,10 @@
       <c r="C19" s="7">
         <v>300</v>
       </c>
-      <c r="D19" s="27"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="28"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="25"/>
       <c r="H19" s="11"/>
       <c r="I19" s="11"/>
       <c r="J19" s="11"/>
@@ -1302,7 +1304,7 @@
       <c r="Q19" s="4"/>
       <c r="S19" s="17"/>
     </row>
-    <row r="20" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="6" t="s">
         <v>30</v>
@@ -1310,14 +1312,14 @@
       <c r="C20" s="7">
         <v>302</v>
       </c>
-      <c r="D20" s="29" t="s">
+      <c r="D20" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="30"/>
-      <c r="F20" s="35" t="s">
+      <c r="E20" s="31"/>
+      <c r="F20" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G20" s="36"/>
+      <c r="G20" s="29"/>
       <c r="H20" s="11"/>
       <c r="I20" s="11"/>
       <c r="J20" s="11"/>
@@ -1332,7 +1334,7 @@
       </c>
       <c r="S20" s="17"/>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
       <c r="B21" s="6" t="s">
         <v>40</v>
@@ -1340,12 +1342,12 @@
       <c r="C21" s="16">
         <v>301</v>
       </c>
-      <c r="D21" s="29" t="s">
+      <c r="D21" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="E21" s="30"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="28"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="25"/>
       <c r="H21" s="11"/>
       <c r="I21" s="11"/>
       <c r="J21" s="11"/>
@@ -1360,14 +1362,14 @@
       </c>
       <c r="S21" s="17"/>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
       <c r="B22" s="6"/>
       <c r="C22" s="7"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="28"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="25"/>
       <c r="H22" s="11"/>
       <c r="I22" s="11"/>
       <c r="J22" s="11"/>
@@ -1380,7 +1382,7 @@
       <c r="Q22" s="4"/>
       <c r="S22" s="17"/>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>3</v>
       </c>
@@ -1390,10 +1392,10 @@
       <c r="C23" s="7">
         <v>400</v>
       </c>
-      <c r="D23" s="27"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="28"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="25"/>
       <c r="H23" s="11"/>
       <c r="I23" s="11"/>
       <c r="J23" s="11"/>
@@ -1406,7 +1408,7 @@
       <c r="Q23" s="4"/>
       <c r="S23" s="17"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
       <c r="B24" s="6" t="s">
         <v>43</v>
@@ -1414,12 +1416,12 @@
       <c r="C24" s="7">
         <v>401</v>
       </c>
-      <c r="D24" s="27" t="s">
+      <c r="D24" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="E24" s="28"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="38"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="27"/>
       <c r="H24" s="11"/>
       <c r="I24" s="11"/>
       <c r="J24" s="11"/>
@@ -1434,7 +1436,7 @@
       </c>
       <c r="S24" s="17"/>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>45</v>
       </c>
@@ -1444,10 +1446,10 @@
       <c r="C25" s="7">
         <v>500</v>
       </c>
-      <c r="D25" s="27"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="28"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="25"/>
       <c r="H25" s="11"/>
       <c r="I25" s="11"/>
       <c r="J25" s="11"/>
@@ -1460,7 +1462,7 @@
       <c r="Q25" s="4"/>
       <c r="S25" s="17"/>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
       <c r="B26" s="6" t="s">
         <v>46</v>
@@ -1468,12 +1470,12 @@
       <c r="C26" s="7">
         <v>501</v>
       </c>
-      <c r="D26" s="27" t="s">
+      <c r="D26" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="E26" s="28"/>
-      <c r="F26" s="27"/>
-      <c r="G26" s="28"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="25"/>
       <c r="H26" s="11"/>
       <c r="I26" s="11"/>
       <c r="J26" s="11"/>
@@ -1488,14 +1490,14 @@
       </c>
       <c r="S26" s="17"/>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="7"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="28"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="25"/>
       <c r="H27" s="8"/>
       <c r="I27" s="8"/>
       <c r="J27" s="8"/>
@@ -1508,14 +1510,14 @@
       <c r="Q27" s="4"/>
       <c r="S27" s="17"/>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="6"/>
       <c r="C28" s="7"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="28"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="25"/>
       <c r="H28" s="8"/>
       <c r="I28" s="8"/>
       <c r="J28" s="8"/>
@@ -1528,67 +1530,74 @@
       <c r="Q28" s="4"/>
       <c r="S28" s="17"/>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D29" s="2"/>
-      <c r="S29" s="19"/>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A30" s="20"/>
-      <c r="S30" s="19"/>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A31" s="20" t="s">
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A30" s="19"/>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A31" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="S31" s="19"/>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A32" s="20" t="s">
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A32" s="19" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="20"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="20" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="19"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="19" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="20"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="20"/>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="20"/>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="20"/>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="20"/>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="20"/>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" s="19"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" s="19"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" s="19"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" s="19"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="H3:O3"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
     <mergeCell ref="F15:G15"/>
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="F21:G21"/>
@@ -1605,28 +1614,20 @@
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="H3:O3"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="75" orientation="landscape" r:id="rId1"/>
@@ -1634,6 +1635,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100CA7F42331C2C26418517DD699E6CB751" ma:contentTypeVersion="8" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="2144a4f294ff69055376aff841bdaa8a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8e441a56-0832-4542-9714-47bfe0559f5f" xmlns:ns3="c1bd8b98-cc9e-46a6-b71b-104d794fef93" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4106c1069881d73dc50bd56f9b52ae75" ns2:_="" ns3:_="">
     <xsd:import namespace="8e441a56-0832-4542-9714-47bfe0559f5f"/>
@@ -1824,15 +1834,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1840,6 +1841,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48FFC07A-B65A-427B-963B-1F060EF78D23}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F77780E-A18D-4A5C-A363-627F96E03E5F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1854,14 +1863,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48FFC07A-B65A-427B-963B-1F060EF78D23}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
many corrections in Magdeburg
</commit_message>
<xml_diff>
--- a/doc/OPC_Jobs_Proto.xlsx
+++ b/doc/OPC_Jobs_Proto.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\rcll-mps-stations\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F159CF2-5124-46C8-B4A9-0CD619629161}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BC5FAE4-B522-4926-9E4C-B280385B53F3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12744" yWindow="5916" windowWidth="23040" windowHeight="13884" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="34560" windowHeight="18744" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OPCJobs" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="66">
   <si>
     <t>Reset</t>
   </si>
@@ -88,9 +88,6 @@
   </si>
   <si>
     <t>reset</t>
-  </si>
-  <si>
-    <t>red</t>
   </si>
   <si>
     <t>0=off/1=on/2=blink</t>
@@ -215,13 +212,25 @@
   </si>
   <si>
     <t>Action Registers for machine specific Jobs (Band, Cylinders)</t>
+  </si>
+  <si>
+    <t>00000bbb</t>
+  </si>
+  <si>
+    <t>00000ryg</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>Signal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -262,6 +271,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -360,7 +377,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -399,9 +416,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -411,47 +425,57 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -770,10 +794,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S40"/>
+  <dimension ref="A1:S41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" zoomScale="219" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -793,7 +817,7 @@
   <sheetData>
     <row r="1" spans="1:19" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="3.6" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -807,32 +831,32 @@
       <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="37" t="s">
+      <c r="D3" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="34" t="s">
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="32"/>
+      <c r="O3" s="33"/>
+      <c r="P3" s="4" t="s">
         <v>57</v>
-      </c>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35"/>
-      <c r="N3" s="35"/>
-      <c r="O3" s="36"/>
-      <c r="P3" s="4" t="s">
-        <v>58</v>
       </c>
       <c r="Q3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="R3" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="S3" s="33"/>
+      <c r="R3" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="S3" s="26"/>
     </row>
     <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
@@ -840,61 +864,61 @@
       <c r="C4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="36"/>
-      <c r="F4" s="34" t="s">
+      <c r="E4" s="33"/>
+      <c r="F4" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="36"/>
-      <c r="H4" s="23">
+      <c r="G4" s="33"/>
+      <c r="H4" s="22">
         <v>7</v>
       </c>
-      <c r="I4" s="23">
+      <c r="I4" s="22">
         <v>6</v>
       </c>
-      <c r="J4" s="23">
+      <c r="J4" s="22">
         <v>5</v>
       </c>
-      <c r="K4" s="23">
+      <c r="K4" s="22">
         <v>4</v>
       </c>
-      <c r="L4" s="23">
+      <c r="L4" s="22">
         <v>3</v>
       </c>
-      <c r="M4" s="23">
+      <c r="M4" s="22">
         <v>2</v>
       </c>
-      <c r="N4" s="23">
+      <c r="N4" s="22">
         <v>1</v>
       </c>
-      <c r="O4" s="23">
+      <c r="O4" s="22">
         <v>0</v>
       </c>
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
       <c r="R4" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="S4" s="4" t="s">
         <v>55</v>
-      </c>
-      <c r="S4" s="4" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:19" s="1" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="36"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="33"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="10"/>
       <c r="K5" s="10"/>
       <c r="L5" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M5" s="10" t="s">
         <v>12</v>
@@ -908,10 +932,10 @@
       <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
       <c r="R5" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="S5" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -924,10 +948,10 @@
       <c r="C6" s="7">
         <v>0</v>
       </c>
-      <c r="D6" s="24"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="25"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="28"/>
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
@@ -950,12 +974,12 @@
       <c r="C7" s="7">
         <v>10</v>
       </c>
-      <c r="D7" s="24" t="s">
+      <c r="D7" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="25"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="22"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="21"/>
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
       <c r="J7" s="11"/>
@@ -978,10 +1002,10 @@
       <c r="C8" s="16">
         <v>20</v>
       </c>
-      <c r="D8" s="24"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="25"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="28"/>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
@@ -996,20 +1020,20 @@
     </row>
     <row r="9" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="24">
         <v>21</v>
       </c>
-      <c r="C9" s="20">
+      <c r="D9" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="24" t="s">
+      <c r="E9" s="38"/>
+      <c r="F9" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="25"/>
-      <c r="F9" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="G9" s="25"/>
+      <c r="G9" s="38"/>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
@@ -1020,26 +1044,26 @@
       <c r="O9" s="8"/>
       <c r="P9" s="8"/>
       <c r="Q9" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S9" s="17"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
-      <c r="B10" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="16">
+      <c r="B10" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="24">
         <v>22</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="38"/>
+      <c r="F10" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="25"/>
-      <c r="F10" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="G10" s="25"/>
+      <c r="G10" s="38"/>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
@@ -1050,26 +1074,26 @@
       <c r="O10" s="8"/>
       <c r="P10" s="8"/>
       <c r="Q10" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S10" s="17"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
-      <c r="B11" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="16">
+      <c r="B11" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="24">
         <v>23</v>
       </c>
-      <c r="D11" s="24" t="s">
+      <c r="D11" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="38"/>
+      <c r="F11" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="25"/>
-      <c r="F11" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="G11" s="25"/>
+      <c r="G11" s="38"/>
       <c r="H11" s="8"/>
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
@@ -1080,50 +1104,52 @@
       <c r="O11" s="8"/>
       <c r="P11" s="8"/>
       <c r="Q11" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S11" s="18"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="5"/>
+      <c r="B12" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="24">
+        <v>25</v>
+      </c>
+      <c r="D12" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" s="28"/>
+      <c r="F12" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="G12" s="28"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="4"/>
+      <c r="S12" s="18"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B13" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C13" s="7">
         <v>100</v>
       </c>
-      <c r="D12" s="24"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="11"/>
-      <c r="N12" s="11"/>
-      <c r="O12" s="11"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="4"/>
-      <c r="S12" s="17"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A13" s="5"/>
-      <c r="B13" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="7">
-        <v>101</v>
-      </c>
-      <c r="D13" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13" s="25"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="25"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="28"/>
       <c r="H13" s="11"/>
       <c r="I13" s="11"/>
       <c r="J13" s="11"/>
@@ -1133,81 +1159,81 @@
       <c r="N13" s="11"/>
       <c r="O13" s="11"/>
       <c r="P13" s="6"/>
-      <c r="Q13" s="4" t="s">
+      <c r="Q13" s="4"/>
+      <c r="S13" s="17"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A14" s="5"/>
+      <c r="B14" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="7">
+        <v>101</v>
+      </c>
+      <c r="D14" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="28"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S14" s="18"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A15" s="12"/>
+      <c r="B15" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="S13" s="18"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
-      <c r="B14" s="15" t="s">
+      <c r="C15" s="16">
+        <v>102</v>
+      </c>
+      <c r="D15" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="16">
-        <v>102</v>
-      </c>
-      <c r="D14" s="30" t="s">
+      <c r="E15" s="30"/>
+      <c r="F15" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="E14" s="31"/>
-      <c r="F14" s="28" t="s">
+      <c r="G15" s="36"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="13"/>
+      <c r="Q15" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G14" s="29"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="14"/>
-      <c r="P14" s="13"/>
-      <c r="Q14" s="4" t="s">
+      <c r="S15" s="17"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="S14" s="17"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="6" t="s">
+      <c r="B16" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C16" s="7">
         <v>200</v>
       </c>
-      <c r="D15" s="24"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="11"/>
-      <c r="N15" s="11"/>
-      <c r="O15" s="11"/>
-      <c r="P15" s="6"/>
-      <c r="Q15" s="4"/>
-      <c r="S15" s="17"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A16" s="5"/>
-      <c r="B16" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="7">
-        <v>201</v>
-      </c>
-      <c r="D16" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="E16" s="25"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="25"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="28"/>
       <c r="H16" s="11"/>
       <c r="I16" s="11"/>
       <c r="J16" s="11"/>
@@ -1218,24 +1244,22 @@
       <c r="O16" s="11"/>
       <c r="P16" s="6"/>
       <c r="Q16" s="4"/>
-      <c r="S16" s="18"/>
+      <c r="S16" s="17"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
       <c r="B17" s="6" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C17" s="7">
-        <v>202</v>
-      </c>
-      <c r="D17" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="E17" s="31"/>
-      <c r="F17" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="G17" s="29"/>
+        <v>201</v>
+      </c>
+      <c r="D17" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" s="28"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="28"/>
       <c r="H17" s="11"/>
       <c r="I17" s="11"/>
       <c r="J17" s="11"/>
@@ -1245,25 +1269,25 @@
       <c r="N17" s="11"/>
       <c r="O17" s="11"/>
       <c r="P17" s="6"/>
-      <c r="Q17" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="S17" s="17"/>
+      <c r="Q17" s="4"/>
+      <c r="S17" s="18"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="6" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C18" s="7">
-        <v>203</v>
-      </c>
-      <c r="D18" s="24" t="s">
+        <v>202</v>
+      </c>
+      <c r="D18" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="E18" s="25"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="25"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="G18" s="36"/>
       <c r="H18" s="11"/>
       <c r="I18" s="11"/>
       <c r="J18" s="11"/>
@@ -1274,24 +1298,24 @@
       <c r="O18" s="11"/>
       <c r="P18" s="6"/>
       <c r="Q18" s="4" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="S18" s="17"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
-        <v>2</v>
-      </c>
+      <c r="A19" s="5"/>
       <c r="B19" s="6" t="s">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="C19" s="7">
-        <v>300</v>
-      </c>
-      <c r="D19" s="24"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="25"/>
+        <v>203</v>
+      </c>
+      <c r="D19" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" s="28"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="28"/>
       <c r="H19" s="11"/>
       <c r="I19" s="11"/>
       <c r="J19" s="11"/>
@@ -1301,25 +1325,25 @@
       <c r="N19" s="11"/>
       <c r="O19" s="11"/>
       <c r="P19" s="6"/>
-      <c r="Q19" s="4"/>
+      <c r="Q19" s="4" t="s">
+        <v>38</v>
+      </c>
       <c r="S19" s="17"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A20" s="5"/>
+      <c r="A20" s="5" t="s">
+        <v>2</v>
+      </c>
       <c r="B20" s="6" t="s">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="C20" s="7">
-        <v>302</v>
-      </c>
-      <c r="D20" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="E20" s="31"/>
-      <c r="F20" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="G20" s="29"/>
+        <v>300</v>
+      </c>
+      <c r="D20" s="27"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="28"/>
       <c r="H20" s="11"/>
       <c r="I20" s="11"/>
       <c r="J20" s="11"/>
@@ -1329,25 +1353,25 @@
       <c r="N20" s="11"/>
       <c r="O20" s="11"/>
       <c r="P20" s="6"/>
-      <c r="Q20" s="4" t="s">
-        <v>33</v>
-      </c>
+      <c r="Q20" s="4"/>
       <c r="S20" s="17"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
       <c r="B21" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C21" s="16">
-        <v>301</v>
-      </c>
-      <c r="D21" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="E21" s="31"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="25"/>
+        <v>29</v>
+      </c>
+      <c r="C21" s="7">
+        <v>302</v>
+      </c>
+      <c r="D21" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" s="30"/>
+      <c r="F21" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="G21" s="36"/>
       <c r="H21" s="11"/>
       <c r="I21" s="11"/>
       <c r="J21" s="11"/>
@@ -1358,18 +1382,24 @@
       <c r="O21" s="11"/>
       <c r="P21" s="6"/>
       <c r="Q21" s="4" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="S21" s="17"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="25"/>
+      <c r="B22" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="16">
+        <v>301</v>
+      </c>
+      <c r="D22" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="E22" s="30"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="28"/>
       <c r="H22" s="11"/>
       <c r="I22" s="11"/>
       <c r="J22" s="11"/>
@@ -1379,23 +1409,19 @@
       <c r="N22" s="11"/>
       <c r="O22" s="11"/>
       <c r="P22" s="6"/>
-      <c r="Q22" s="4"/>
+      <c r="Q22" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="S22" s="17"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A23" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C23" s="7">
-        <v>400</v>
-      </c>
-      <c r="D23" s="24"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="25"/>
+      <c r="A23" s="5"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="28"/>
       <c r="H23" s="11"/>
       <c r="I23" s="11"/>
       <c r="J23" s="11"/>
@@ -1409,19 +1435,19 @@
       <c r="S23" s="17"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A24" s="5"/>
+      <c r="A24" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="B24" s="6" t="s">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="C24" s="7">
-        <v>401</v>
-      </c>
-      <c r="D24" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="E24" s="25"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="27"/>
+        <v>400</v>
+      </c>
+      <c r="D24" s="27"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="28"/>
       <c r="H24" s="11"/>
       <c r="I24" s="11"/>
       <c r="J24" s="11"/>
@@ -1431,25 +1457,23 @@
       <c r="N24" s="11"/>
       <c r="O24" s="11"/>
       <c r="P24" s="6"/>
-      <c r="Q24" s="4" t="s">
-        <v>44</v>
-      </c>
+      <c r="Q24" s="4"/>
       <c r="S24" s="17"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A25" s="5" t="s">
-        <v>45</v>
-      </c>
+      <c r="A25" s="5"/>
       <c r="B25" s="6" t="s">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="C25" s="7">
-        <v>500</v>
-      </c>
-      <c r="D25" s="24"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="24"/>
-      <c r="G25" s="25"/>
+        <v>401</v>
+      </c>
+      <c r="D25" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="E25" s="28"/>
+      <c r="F25" s="39"/>
+      <c r="G25" s="40"/>
       <c r="H25" s="11"/>
       <c r="I25" s="11"/>
       <c r="J25" s="11"/>
@@ -1459,23 +1483,25 @@
       <c r="N25" s="11"/>
       <c r="O25" s="11"/>
       <c r="P25" s="6"/>
-      <c r="Q25" s="4"/>
+      <c r="Q25" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="S25" s="17"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A26" s="5"/>
+      <c r="A26" s="5" t="s">
+        <v>44</v>
+      </c>
       <c r="B26" s="6" t="s">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="C26" s="7">
-        <v>501</v>
-      </c>
-      <c r="D26" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="E26" s="25"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="25"/>
+        <v>500</v>
+      </c>
+      <c r="D26" s="27"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="28"/>
       <c r="H26" s="11"/>
       <c r="I26" s="11"/>
       <c r="J26" s="11"/>
@@ -1485,39 +1511,45 @@
       <c r="N26" s="11"/>
       <c r="O26" s="11"/>
       <c r="P26" s="6"/>
-      <c r="Q26" s="4" t="s">
-        <v>48</v>
-      </c>
+      <c r="Q26" s="4"/>
       <c r="S26" s="17"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="25"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="8"/>
-      <c r="M27" s="8"/>
-      <c r="N27" s="8"/>
-      <c r="O27" s="8"/>
-      <c r="P27" s="8"/>
-      <c r="Q27" s="4"/>
+      <c r="B27" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27" s="7">
+        <v>501</v>
+      </c>
+      <c r="D27" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="E27" s="28"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="11"/>
+      <c r="M27" s="11"/>
+      <c r="N27" s="11"/>
+      <c r="O27" s="11"/>
+      <c r="P27" s="6"/>
+      <c r="Q27" s="4" t="s">
+        <v>47</v>
+      </c>
       <c r="S27" s="17"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
-      <c r="B28" s="6"/>
+      <c r="B28" s="5"/>
       <c r="C28" s="7"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="25"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="28"/>
       <c r="H28" s="8"/>
       <c r="I28" s="8"/>
       <c r="J28" s="8"/>
@@ -1531,36 +1563,53 @@
       <c r="S28" s="17"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="D29" s="2"/>
+      <c r="A29" s="5"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="8"/>
+      <c r="M29" s="8"/>
+      <c r="N29" s="8"/>
+      <c r="O29" s="8"/>
+      <c r="P29" s="8"/>
+      <c r="Q29" s="4"/>
+      <c r="S29" s="17"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A30" s="19"/>
+      <c r="D30" s="2"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A31" s="19" t="s">
-        <v>59</v>
-      </c>
+      <c r="A31" s="19"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" s="19" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="19"/>
+      <c r="A33" s="19" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" s="19" t="s">
-        <v>61</v>
-      </c>
+      <c r="A34" s="19"/>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" s="19"/>
+      <c r="A36" s="19" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" s="19"/>
@@ -1574,60 +1623,65 @@
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" s="19"/>
     </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" s="19"/>
+    </row>
   </sheetData>
-  <mergeCells count="52">
+  <mergeCells count="54">
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
     <mergeCell ref="R3:S3"/>
     <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D12:E12"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
     <mergeCell ref="H3:O3"/>
     <mergeCell ref="D3:G3"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
     <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="D12:E12"/>
     <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="75" orientation="landscape" r:id="rId1"/>
@@ -1635,15 +1689,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100CA7F42331C2C26418517DD699E6CB751" ma:contentTypeVersion="8" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="2144a4f294ff69055376aff841bdaa8a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8e441a56-0832-4542-9714-47bfe0559f5f" xmlns:ns3="c1bd8b98-cc9e-46a6-b71b-104d794fef93" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4106c1069881d73dc50bd56f9b52ae75" ns2:_="" ns3:_="">
     <xsd:import namespace="8e441a56-0832-4542-9714-47bfe0559f5f"/>
@@ -1834,6 +1879,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1841,14 +1895,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48FFC07A-B65A-427B-963B-1F060EF78D23}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F77780E-A18D-4A5C-A363-627F96E03E5F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1863,6 +1909,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48FFC07A-B65A-427B-963B-1F060EF78D23}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Updated Version and Documents
- quickstart guide
- MPS Software V1.1 (Barcode as Integer and new OPC-Version-Register)
</commit_message>
<xml_diff>
--- a/doc/OPC_Jobs_Proto.xlsx
+++ b/doc/OPC_Jobs_Proto.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\rcll-mps-stations\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\SysTech - Dokumente\01_Projekte\00_RoboCup\07_MPS_RoboCupStations\_GIT\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BC5FAE4-B522-4926-9E4C-B280385B53F3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4094BA88-DB82-47CB-BE36-CECDFFF708F5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="34560" windowHeight="18744" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OPCJobs" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="68">
   <si>
     <t>Reset</t>
   </si>
@@ -224,13 +224,19 @@
   </si>
   <si>
     <t>Signal</t>
+  </si>
+  <si>
+    <t>String[4]</t>
+  </si>
+  <si>
+    <t>Prg_Version</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -271,14 +277,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="0" tint="-0.34998626667073579"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -377,7 +375,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -425,28 +423,33 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -459,23 +462,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -794,34 +782,34 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S41"/>
+  <dimension ref="A1:T41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="219" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="S9" sqref="S9"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12:E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" customWidth="1"/>
-    <col min="3" max="3" width="7.5546875" customWidth="1"/>
-    <col min="4" max="4" width="15.88671875" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" customWidth="1"/>
-    <col min="6" max="6" width="10.5546875" customWidth="1"/>
-    <col min="7" max="7" width="11.109375" customWidth="1"/>
-    <col min="8" max="15" width="2.109375" style="9" customWidth="1"/>
-    <col min="16" max="16" width="9.109375" customWidth="1"/>
-    <col min="17" max="17" width="17.88671875" customWidth="1"/>
-    <col min="18" max="19" width="8.109375" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" customWidth="1"/>
+    <col min="8" max="15" width="2.140625" style="9" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" customWidth="1"/>
+    <col min="17" max="17" width="17.85546875" customWidth="1"/>
+    <col min="18" max="19" width="8.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="3.6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:19" ht="29.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" ht="3.6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:20" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -831,47 +819,48 @@
       <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="34" t="s">
+      <c r="D3" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="31" t="s">
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="32"/>
-      <c r="M3" s="32"/>
-      <c r="N3" s="32"/>
-      <c r="O3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="33"/>
+      <c r="N3" s="33"/>
+      <c r="O3" s="34"/>
       <c r="P3" s="4" t="s">
         <v>57</v>
       </c>
       <c r="Q3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="R3" s="25" t="s">
+      <c r="R3" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="S3" s="26"/>
-    </row>
-    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S3" s="36"/>
+      <c r="T3" s="36"/>
+    </row>
+    <row r="4" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="33"/>
-      <c r="F4" s="31" t="s">
+      <c r="E4" s="34"/>
+      <c r="F4" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="33"/>
+      <c r="G4" s="34"/>
       <c r="H4" s="22">
         <v>7</v>
       </c>
@@ -904,15 +893,18 @@
       <c r="S4" s="4" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" s="1" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T4" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" s="1" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="33"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="34"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="10"/>
@@ -937,8 +929,11 @@
       <c r="S5" s="4" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="T5" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>15</v>
       </c>
@@ -948,10 +943,10 @@
       <c r="C6" s="7">
         <v>0</v>
       </c>
-      <c r="D6" s="27"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="28"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="24"/>
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
@@ -964,7 +959,7 @@
       <c r="Q6" s="4"/>
       <c r="S6" s="17"/>
     </row>
-    <row r="7" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>15</v>
       </c>
@@ -974,10 +969,10 @@
       <c r="C7" s="7">
         <v>10</v>
       </c>
-      <c r="D7" s="27" t="s">
+      <c r="D7" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="28"/>
+      <c r="E7" s="24"/>
       <c r="F7" s="20"/>
       <c r="G7" s="21"/>
       <c r="H7" s="11"/>
@@ -992,7 +987,7 @@
       <c r="Q7" s="4"/>
       <c r="S7" s="17"/>
     </row>
-    <row r="8" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>19</v>
       </c>
@@ -1002,10 +997,10 @@
       <c r="C8" s="16">
         <v>20</v>
       </c>
-      <c r="D8" s="27"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="28"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="24"/>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
@@ -1018,22 +1013,22 @@
       <c r="Q8" s="4"/>
       <c r="S8" s="17"/>
     </row>
-    <row r="9" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="C9" s="24">
+      <c r="C9" s="16">
         <v>21</v>
       </c>
-      <c r="D9" s="37" t="s">
+      <c r="D9" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="38"/>
-      <c r="F9" s="37" t="s">
+      <c r="E9" s="30"/>
+      <c r="F9" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="38"/>
+      <c r="G9" s="30"/>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
@@ -1048,22 +1043,22 @@
       </c>
       <c r="S9" s="17"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="24">
+      <c r="C10" s="16">
         <v>22</v>
       </c>
-      <c r="D10" s="37" t="s">
+      <c r="D10" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="38"/>
-      <c r="F10" s="37" t="s">
+      <c r="E10" s="30"/>
+      <c r="F10" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="38"/>
+      <c r="G10" s="30"/>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
@@ -1078,22 +1073,22 @@
       </c>
       <c r="S10" s="17"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="24">
+      <c r="C11" s="16">
         <v>23</v>
       </c>
-      <c r="D11" s="37" t="s">
+      <c r="D11" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="38"/>
-      <c r="F11" s="37" t="s">
+      <c r="E11" s="30"/>
+      <c r="F11" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="G11" s="38"/>
+      <c r="G11" s="30"/>
       <c r="H11" s="8"/>
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
@@ -1108,22 +1103,22 @@
       </c>
       <c r="S11" s="18"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="C12" s="24">
+      <c r="C12" s="16">
         <v>25</v>
       </c>
-      <c r="D12" s="27" t="s">
+      <c r="D12" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="E12" s="28"/>
-      <c r="F12" s="27" t="s">
+      <c r="E12" s="30"/>
+      <c r="F12" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="G12" s="28"/>
+      <c r="G12" s="30"/>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
@@ -1136,7 +1131,7 @@
       <c r="Q12" s="4"/>
       <c r="S12" s="18"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>1</v>
       </c>
@@ -1146,10 +1141,10 @@
       <c r="C13" s="7">
         <v>100</v>
       </c>
-      <c r="D13" s="27"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="28"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="24"/>
       <c r="H13" s="11"/>
       <c r="I13" s="11"/>
       <c r="J13" s="11"/>
@@ -1162,7 +1157,7 @@
       <c r="Q13" s="4"/>
       <c r="S13" s="17"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="6" t="s">
         <v>26</v>
@@ -1170,12 +1165,12 @@
       <c r="C14" s="7">
         <v>101</v>
       </c>
-      <c r="D14" s="27" t="s">
+      <c r="D14" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="28"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="28"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="24"/>
       <c r="H14" s="11"/>
       <c r="I14" s="11"/>
       <c r="J14" s="11"/>
@@ -1190,7 +1185,7 @@
       </c>
       <c r="S14" s="18"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
       <c r="B15" s="15" t="s">
         <v>29</v>
@@ -1202,10 +1197,10 @@
         <v>30</v>
       </c>
       <c r="E15" s="30"/>
-      <c r="F15" s="35" t="s">
+      <c r="F15" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="G15" s="36"/>
+      <c r="G15" s="28"/>
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
       <c r="J15" s="14"/>
@@ -1220,7 +1215,7 @@
       </c>
       <c r="S15" s="17"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>33</v>
       </c>
@@ -1230,10 +1225,10 @@
       <c r="C16" s="7">
         <v>200</v>
       </c>
-      <c r="D16" s="27"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="28"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="24"/>
       <c r="H16" s="11"/>
       <c r="I16" s="11"/>
       <c r="J16" s="11"/>
@@ -1246,7 +1241,7 @@
       <c r="Q16" s="4"/>
       <c r="S16" s="17"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="6" t="s">
         <v>34</v>
@@ -1254,12 +1249,12 @@
       <c r="C17" s="7">
         <v>201</v>
       </c>
-      <c r="D17" s="27" t="s">
+      <c r="D17" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="E17" s="28"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="28"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="24"/>
       <c r="H17" s="11"/>
       <c r="I17" s="11"/>
       <c r="J17" s="11"/>
@@ -1272,7 +1267,7 @@
       <c r="Q17" s="4"/>
       <c r="S17" s="18"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="6" t="s">
         <v>29</v>
@@ -1284,10 +1279,10 @@
         <v>36</v>
       </c>
       <c r="E18" s="30"/>
-      <c r="F18" s="35" t="s">
+      <c r="F18" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="G18" s="36"/>
+      <c r="G18" s="28"/>
       <c r="H18" s="11"/>
       <c r="I18" s="11"/>
       <c r="J18" s="11"/>
@@ -1302,7 +1297,7 @@
       </c>
       <c r="S18" s="17"/>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="6" t="s">
         <v>37</v>
@@ -1310,12 +1305,12 @@
       <c r="C19" s="7">
         <v>203</v>
       </c>
-      <c r="D19" s="27" t="s">
+      <c r="D19" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="E19" s="28"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="28"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="24"/>
       <c r="H19" s="11"/>
       <c r="I19" s="11"/>
       <c r="J19" s="11"/>
@@ -1330,7 +1325,7 @@
       </c>
       <c r="S19" s="17"/>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>2</v>
       </c>
@@ -1340,10 +1335,10 @@
       <c r="C20" s="7">
         <v>300</v>
       </c>
-      <c r="D20" s="27"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="28"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="24"/>
       <c r="H20" s="11"/>
       <c r="I20" s="11"/>
       <c r="J20" s="11"/>
@@ -1356,7 +1351,7 @@
       <c r="Q20" s="4"/>
       <c r="S20" s="17"/>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="6" t="s">
         <v>29</v>
@@ -1368,10 +1363,10 @@
         <v>36</v>
       </c>
       <c r="E21" s="30"/>
-      <c r="F21" s="35" t="s">
+      <c r="F21" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="G21" s="36"/>
+      <c r="G21" s="28"/>
       <c r="H21" s="11"/>
       <c r="I21" s="11"/>
       <c r="J21" s="11"/>
@@ -1386,7 +1381,7 @@
       </c>
       <c r="S21" s="17"/>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="6" t="s">
         <v>39</v>
@@ -1398,8 +1393,8 @@
         <v>40</v>
       </c>
       <c r="E22" s="30"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="28"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="24"/>
       <c r="H22" s="11"/>
       <c r="I22" s="11"/>
       <c r="J22" s="11"/>
@@ -1414,14 +1409,14 @@
       </c>
       <c r="S22" s="17"/>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="6"/>
       <c r="C23" s="7"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="28"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="24"/>
       <c r="H23" s="11"/>
       <c r="I23" s="11"/>
       <c r="J23" s="11"/>
@@ -1434,7 +1429,7 @@
       <c r="Q23" s="4"/>
       <c r="S23" s="17"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>3</v>
       </c>
@@ -1444,10 +1439,10 @@
       <c r="C24" s="7">
         <v>400</v>
       </c>
-      <c r="D24" s="27"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="28"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="24"/>
       <c r="H24" s="11"/>
       <c r="I24" s="11"/>
       <c r="J24" s="11"/>
@@ -1460,7 +1455,7 @@
       <c r="Q24" s="4"/>
       <c r="S24" s="17"/>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="6" t="s">
         <v>42</v>
@@ -1468,12 +1463,12 @@
       <c r="C25" s="7">
         <v>401</v>
       </c>
-      <c r="D25" s="27" t="s">
+      <c r="D25" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="E25" s="28"/>
-      <c r="F25" s="39"/>
-      <c r="G25" s="40"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="26"/>
       <c r="H25" s="11"/>
       <c r="I25" s="11"/>
       <c r="J25" s="11"/>
@@ -1488,7 +1483,7 @@
       </c>
       <c r="S25" s="17"/>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>44</v>
       </c>
@@ -1498,10 +1493,10 @@
       <c r="C26" s="7">
         <v>500</v>
       </c>
-      <c r="D26" s="27"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="27"/>
-      <c r="G26" s="28"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="24"/>
       <c r="H26" s="11"/>
       <c r="I26" s="11"/>
       <c r="J26" s="11"/>
@@ -1514,7 +1509,7 @@
       <c r="Q26" s="4"/>
       <c r="S26" s="17"/>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="6" t="s">
         <v>45</v>
@@ -1522,12 +1517,12 @@
       <c r="C27" s="7">
         <v>501</v>
       </c>
-      <c r="D27" s="27" t="s">
+      <c r="D27" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="E27" s="28"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="28"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="24"/>
       <c r="H27" s="11"/>
       <c r="I27" s="11"/>
       <c r="J27" s="11"/>
@@ -1542,14 +1537,14 @@
       </c>
       <c r="S27" s="17"/>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="7"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="28"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="24"/>
       <c r="H28" s="8"/>
       <c r="I28" s="8"/>
       <c r="J28" s="8"/>
@@ -1562,14 +1557,14 @@
       <c r="Q28" s="4"/>
       <c r="S28" s="17"/>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="6"/>
       <c r="C29" s="7"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="28"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="28"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="24"/>
       <c r="H29" s="8"/>
       <c r="I29" s="8"/>
       <c r="J29" s="8"/>
@@ -1582,66 +1577,76 @@
       <c r="Q29" s="4"/>
       <c r="S29" s="17"/>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D30" s="2"/>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="19"/>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="19" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="19"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="19" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="19" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="19"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="19"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="19"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="19"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="R3:T3"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="H3:O3"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
     <mergeCell ref="F16:G16"/>
     <mergeCell ref="F21:G21"/>
     <mergeCell ref="F22:G22"/>
@@ -1658,30 +1663,20 @@
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="F14:G14"/>
     <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="H3:O3"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="75" orientation="landscape" r:id="rId1"/>
@@ -1689,24 +1684,35 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100CA7F42331C2C26418517DD699E6CB751" ma:contentTypeVersion="8" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="2144a4f294ff69055376aff841bdaa8a">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8e441a56-0832-4542-9714-47bfe0559f5f" xmlns:ns3="c1bd8b98-cc9e-46a6-b71b-104d794fef93" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4106c1069881d73dc50bd56f9b52ae75" ns2:_="" ns3:_="">
-    <xsd:import namespace="8e441a56-0832-4542-9714-47bfe0559f5f"/>
-    <xsd:import namespace="c1bd8b98-cc9e-46a6-b71b-104d794fef93"/>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100518FA119520CC8428F89027E7E23B6BC" ma:contentTypeVersion="10" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="525c35728d505c3eded287358983ca7d">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9defabeb-577e-409c-8009-be238c901e13" xmlns:ns3="900e6cd2-e6b4-4a77-8178-c82fa39f99ac" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="eaddf080a51846a57337f9b0d92d87ba" ns2:_="" ns3:_="">
+    <xsd:import namespace="9defabeb-577e-409c-8009-be238c901e13"/>
+    <xsd:import namespace="900e6cd2-e6b4-4a77-8178-c82fa39f99ac"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element name="documentManagement">
             <xsd:complexType>
               <xsd:all>
-                <xsd:element ref="ns2:SharedWithUsers" minOccurs="0"/>
-                <xsd:element ref="ns2:SharedWithDetails" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceAutoTags" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceLocation" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -1714,10 +1720,56 @@
       </xsd:complexType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="8e441a56-0832-4542-9714-47bfe0559f5f" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="9defabeb-577e-409c-8009-be238c901e13" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="8" nillable="true" ma:displayName="Freigegeben für" ma:internalName="SharedWithUsers" ma:readOnly="true">
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="10" nillable="true" ma:displayName="MediaServiceAutoTags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="11" nillable="true" ma:displayName="MediaServiceOCR" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="12" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="13" nillable="true" ma:displayName="MediaServiceLocation" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="16" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="17" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="900e6cd2-e6b4-4a77-8178-c82fa39f99ac" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="14" nillable="true" ma:displayName="Freigegeben für" ma:internalName="SharedWithUsers" ma:readOnly="true">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:UserMulti">
@@ -1736,43 +1788,7 @@
         </xsd:complexContent>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="9" nillable="true" ma:displayName="Freigegeben für - Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="c1bd8b98-cc9e-46a6-b71b-104d794fef93" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="10" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="11" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceAutoTags" ma:index="12" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="13" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceLocation" ma:index="14" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="15" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+    <xsd:element name="SharedWithDetails" ma:index="15" nillable="true" ma:displayName="Freigegeben für - Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
@@ -1879,15 +1895,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1895,28 +1902,28 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F77780E-A18D-4A5C-A363-627F96E03E5F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48FFC07A-B65A-427B-963B-1F060EF78D23}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B08C82FB-AE2A-4BAA-9E62-2E21FAC4D1E1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
     <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="8e441a56-0832-4542-9714-47bfe0559f5f"/>
-    <ds:schemaRef ds:uri="c1bd8b98-cc9e-46a6-b71b-104d794fef93"/>
+    <ds:schemaRef ds:uri="9defabeb-577e-409c-8009-be238c901e13"/>
+    <ds:schemaRef ds:uri="900e6cd2-e6b4-4a77-8178-c82fa39f99ac"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48FFC07A-B65A-427B-963B-1F060EF78D23}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>